<commit_message>
COMPROBACION DE DATO WF Y PAGO UNICO OBSERVADOS
</commit_message>
<xml_diff>
--- a/mapeo WF.xlsx
+++ b/mapeo WF.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="3555"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="3555" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -732,10 +732,10 @@
     <t>Seguridad.Rol</t>
   </si>
   <si>
-    <t>No iguala con la tabla destino</t>
-  </si>
-  <si>
     <t xml:space="preserve">5 solicitudes, uno por cada concepto, en cada caso los datos van variando según el orden en que se los a listado                                                                                                    25 registros </t>
+  </si>
+  <si>
+    <t>No iguala con la tabla destino (68 registros)</t>
   </si>
 </sst>
 </file>
@@ -929,39 +929,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -980,14 +947,38 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -997,6 +988,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1280,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,14 +1296,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1328,7 +1328,7 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="38" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1343,13 +1343,13 @@
       <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="39" t="s">
         <v>136</v>
       </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="27"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1362,11 +1362,11 @@
       <c r="E4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="34"/>
+      <c r="F4" s="40"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1379,11 +1379,11 @@
       <c r="E5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="34"/>
+      <c r="F5" s="40"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="27"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1396,11 +1396,11 @@
       <c r="E6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1413,11 +1413,11 @@
       <c r="E7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="40"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1430,11 +1430,11 @@
       <c r="E8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1447,11 +1447,11 @@
       <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="27"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1464,11 +1464,11 @@
       <c r="E10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1481,11 +1481,11 @@
       <c r="E11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="34"/>
+      <c r="F11" s="40"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1498,11 +1498,11 @@
       <c r="E12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="34"/>
+      <c r="F12" s="40"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="27"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1515,11 +1515,11 @@
       <c r="E13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="34"/>
+      <c r="F13" s="40"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="27"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1532,11 +1532,11 @@
       <c r="E14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="34"/>
+      <c r="F14" s="40"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1549,11 +1549,11 @@
       <c r="E15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="34"/>
+      <c r="F15" s="40"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="28"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="9" t="s">
         <v>18</v>
       </c>
@@ -1566,11 +1566,11 @@
       <c r="E16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="35"/>
+      <c r="F16" s="41"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="11" t="s">
@@ -1585,7 +1585,7 @@
       <c r="E17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="36" t="s">
+      <c r="F17" s="25" t="s">
         <v>141</v>
       </c>
       <c r="G17" s="12">
@@ -1593,7 +1593,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="5" t="s">
         <v>25</v>
       </c>
@@ -1606,13 +1606,13 @@
       <c r="E18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="37"/>
+      <c r="F18" s="26"/>
       <c r="G18" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="27"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
@@ -1625,13 +1625,13 @@
       <c r="E19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="37"/>
+      <c r="F19" s="26"/>
       <c r="G19" s="7" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="5" t="s">
         <v>8</v>
       </c>
@@ -1644,13 +1644,13 @@
       <c r="E20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="37"/>
+      <c r="F20" s="26"/>
       <c r="G20" s="8" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="27"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="5" t="s">
         <v>9</v>
       </c>
@@ -1663,13 +1663,13 @@
       <c r="E21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="37"/>
+      <c r="F21" s="26"/>
       <c r="G21" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="27"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="5" t="s">
         <v>10</v>
       </c>
@@ -1682,13 +1682,13 @@
       <c r="E22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="26"/>
       <c r="G22" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="27"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
@@ -1701,13 +1701,13 @@
       <c r="E23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="37"/>
+      <c r="F23" s="26"/>
       <c r="G23" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="27"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
@@ -1720,13 +1720,13 @@
       <c r="E24" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="37"/>
+      <c r="F24" s="26"/>
       <c r="G24" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="27"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="5" t="s">
         <v>15</v>
       </c>
@@ -1739,13 +1739,13 @@
       <c r="E25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="37"/>
+      <c r="F25" s="26"/>
       <c r="G25" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="27"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1758,13 +1758,13 @@
       <c r="E26" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="37"/>
+      <c r="F26" s="26"/>
       <c r="G26" s="8">
         <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="27"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="5" t="s">
         <v>17</v>
       </c>
@@ -1777,13 +1777,13 @@
       <c r="E27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="37"/>
+      <c r="F27" s="26"/>
       <c r="G27" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="27"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="5" t="s">
         <v>26</v>
       </c>
@@ -1796,13 +1796,13 @@
       <c r="E28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="37"/>
+      <c r="F28" s="26"/>
       <c r="G28" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="27"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="5" t="s">
         <v>27</v>
       </c>
@@ -1815,13 +1815,13 @@
       <c r="E29" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="37"/>
+      <c r="F29" s="26"/>
       <c r="G29" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="27"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="5" t="s">
         <v>28</v>
       </c>
@@ -1834,13 +1834,13 @@
       <c r="E30" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="37"/>
+      <c r="F30" s="26"/>
       <c r="G30" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="27"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="5" t="s">
         <v>29</v>
       </c>
@@ -1853,13 +1853,13 @@
       <c r="E31" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="37"/>
+      <c r="F31" s="26"/>
       <c r="G31" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="27"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="5" t="s">
         <v>30</v>
       </c>
@@ -1872,13 +1872,13 @@
       <c r="E32" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F32" s="37"/>
+      <c r="F32" s="26"/>
       <c r="G32" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="27"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="5" t="s">
         <v>31</v>
       </c>
@@ -1891,13 +1891,13 @@
       <c r="E33" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="37"/>
+      <c r="F33" s="26"/>
       <c r="G33" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="28"/>
+      <c r="A34" s="33"/>
       <c r="B34" s="9" t="s">
         <v>32</v>
       </c>
@@ -1910,13 +1910,13 @@
       <c r="E34" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F34" s="38"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="31" t="s">
         <v>45</v>
       </c>
       <c r="B35" s="11" t="s">
@@ -1931,7 +1931,7 @@
       <c r="E35" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="36" t="s">
+      <c r="F35" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G35" s="12">
@@ -1939,7 +1939,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="27"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="5" t="s">
         <v>35</v>
       </c>
@@ -1952,13 +1952,13 @@
       <c r="E36" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F36" s="37"/>
+      <c r="F36" s="26"/>
       <c r="G36" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="27"/>
+      <c r="A37" s="32"/>
       <c r="B37" s="5" t="s">
         <v>25</v>
       </c>
@@ -1971,13 +1971,13 @@
       <c r="E37" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F37" s="37"/>
+      <c r="F37" s="26"/>
       <c r="G37" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="27"/>
+      <c r="A38" s="32"/>
       <c r="B38" s="5" t="s">
         <v>11</v>
       </c>
@@ -1990,13 +1990,13 @@
       <c r="E38" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F38" s="37"/>
+      <c r="F38" s="26"/>
       <c r="G38" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A39" s="27"/>
+      <c r="A39" s="32"/>
       <c r="B39" s="5" t="s">
         <v>36</v>
       </c>
@@ -2009,13 +2009,13 @@
       <c r="E39" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F39" s="37"/>
+      <c r="F39" s="26"/>
       <c r="G39" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A40" s="27"/>
+      <c r="A40" s="32"/>
       <c r="B40" s="5" t="s">
         <v>37</v>
       </c>
@@ -2028,13 +2028,13 @@
       <c r="E40" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F40" s="37"/>
+      <c r="F40" s="26"/>
       <c r="G40" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A41" s="27"/>
+      <c r="A41" s="32"/>
       <c r="B41" s="5" t="s">
         <v>38</v>
       </c>
@@ -2047,13 +2047,13 @@
       <c r="E41" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F41" s="37"/>
+      <c r="F41" s="26"/>
       <c r="G41" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="27"/>
+      <c r="A42" s="32"/>
       <c r="B42" s="5" t="s">
         <v>39</v>
       </c>
@@ -2066,13 +2066,13 @@
       <c r="E42" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F42" s="37"/>
+      <c r="F42" s="26"/>
       <c r="G42" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="27"/>
+      <c r="A43" s="32"/>
       <c r="B43" s="5" t="s">
         <v>40</v>
       </c>
@@ -2085,13 +2085,13 @@
       <c r="E43" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="37"/>
+      <c r="F43" s="26"/>
       <c r="G43" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="27"/>
+      <c r="A44" s="32"/>
       <c r="B44" s="5" t="s">
         <v>41</v>
       </c>
@@ -2104,13 +2104,13 @@
       <c r="E44" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F44" s="37"/>
+      <c r="F44" s="26"/>
       <c r="G44" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="27"/>
+      <c r="A45" s="32"/>
       <c r="B45" s="5" t="s">
         <v>42</v>
       </c>
@@ -2123,13 +2123,13 @@
       <c r="E45" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F45" s="37"/>
+      <c r="F45" s="26"/>
       <c r="G45" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A46" s="27"/>
+      <c r="A46" s="32"/>
       <c r="B46" s="5" t="s">
         <v>43</v>
       </c>
@@ -2142,13 +2142,13 @@
       <c r="E46" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F46" s="37"/>
+      <c r="F46" s="26"/>
       <c r="G46" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="28"/>
+      <c r="A47" s="33"/>
       <c r="B47" s="9" t="s">
         <v>44</v>
       </c>
@@ -2161,13 +2161,13 @@
       <c r="E47" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="38"/>
+      <c r="F47" s="27"/>
       <c r="G47" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="33" x14ac:dyDescent="0.3">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="31" t="s">
         <v>103</v>
       </c>
       <c r="B48" s="11" t="s">
@@ -2182,13 +2182,13 @@
       <c r="E48" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F48" s="36" t="s">
+      <c r="F48" s="25" t="s">
         <v>138</v>
       </c>
       <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A49" s="27"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="5" t="s">
         <v>6</v>
       </c>
@@ -2201,11 +2201,11 @@
       <c r="E49" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F49" s="37"/>
+      <c r="F49" s="26"/>
       <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A50" s="27"/>
+      <c r="A50" s="32"/>
       <c r="B50" s="5" t="s">
         <v>8</v>
       </c>
@@ -2218,11 +2218,11 @@
       <c r="E50" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F50" s="37"/>
+      <c r="F50" s="26"/>
       <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A51" s="27"/>
+      <c r="A51" s="32"/>
       <c r="B51" s="5" t="s">
         <v>59</v>
       </c>
@@ -2235,11 +2235,11 @@
       <c r="E51" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F51" s="37"/>
+      <c r="F51" s="26"/>
       <c r="G51" s="7"/>
     </row>
     <row r="52" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A52" s="27"/>
+      <c r="A52" s="32"/>
       <c r="B52" s="5" t="s">
         <v>98</v>
       </c>
@@ -2252,11 +2252,11 @@
       <c r="E52" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F52" s="37"/>
+      <c r="F52" s="26"/>
       <c r="G52" s="7"/>
     </row>
     <row r="53" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A53" s="27"/>
+      <c r="A53" s="32"/>
       <c r="B53" s="5" t="s">
         <v>99</v>
       </c>
@@ -2269,11 +2269,11 @@
       <c r="E53" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F53" s="37"/>
+      <c r="F53" s="26"/>
       <c r="G53" s="7"/>
     </row>
     <row r="54" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A54" s="27"/>
+      <c r="A54" s="32"/>
       <c r="B54" s="5" t="s">
         <v>100</v>
       </c>
@@ -2286,11 +2286,11 @@
       <c r="E54" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F54" s="37"/>
+      <c r="F54" s="26"/>
       <c r="G54" s="7"/>
     </row>
     <row r="55" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A55" s="27"/>
+      <c r="A55" s="32"/>
       <c r="B55" s="5" t="s">
         <v>101</v>
       </c>
@@ -2303,11 +2303,11 @@
       <c r="E55" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F55" s="37"/>
+      <c r="F55" s="26"/>
       <c r="G55" s="7"/>
     </row>
     <row r="56" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="28"/>
+      <c r="A56" s="33"/>
       <c r="B56" s="9" t="s">
         <v>102</v>
       </c>
@@ -2320,11 +2320,11 @@
       <c r="E56" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F56" s="38"/>
+      <c r="F56" s="27"/>
       <c r="G56" s="7"/>
     </row>
     <row r="57" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A57" s="29" t="s">
+      <c r="A57" s="31" t="s">
         <v>110</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -2339,13 +2339,13 @@
       <c r="E57" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F57" s="36" t="s">
+      <c r="F57" s="25" t="s">
         <v>137</v>
       </c>
       <c r="G57" s="7"/>
     </row>
     <row r="58" spans="1:7" ht="33" x14ac:dyDescent="0.3">
-      <c r="A58" s="27"/>
+      <c r="A58" s="32"/>
       <c r="B58" s="5" t="s">
         <v>58</v>
       </c>
@@ -2358,11 +2358,11 @@
       <c r="E58" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F58" s="37"/>
+      <c r="F58" s="26"/>
       <c r="G58" s="7"/>
     </row>
     <row r="59" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A59" s="27"/>
+      <c r="A59" s="32"/>
       <c r="B59" s="5" t="s">
         <v>105</v>
       </c>
@@ -2375,11 +2375,11 @@
       <c r="E59" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F59" s="37"/>
+      <c r="F59" s="26"/>
       <c r="G59" s="7"/>
     </row>
     <row r="60" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A60" s="27"/>
+      <c r="A60" s="32"/>
       <c r="B60" s="5" t="s">
         <v>106</v>
       </c>
@@ -2392,11 +2392,11 @@
       <c r="E60" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F60" s="37"/>
+      <c r="F60" s="26"/>
       <c r="G60" s="7"/>
     </row>
     <row r="61" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A61" s="27"/>
+      <c r="A61" s="32"/>
       <c r="B61" s="5" t="s">
         <v>107</v>
       </c>
@@ -2409,11 +2409,11 @@
       <c r="E61" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F61" s="37"/>
+      <c r="F61" s="26"/>
       <c r="G61" s="7"/>
     </row>
     <row r="62" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A62" s="27"/>
+      <c r="A62" s="32"/>
       <c r="B62" s="5" t="s">
         <v>108</v>
       </c>
@@ -2426,11 +2426,11 @@
       <c r="E62" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F62" s="37"/>
+      <c r="F62" s="26"/>
       <c r="G62" s="7"/>
     </row>
     <row r="63" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A63" s="27"/>
+      <c r="A63" s="32"/>
       <c r="B63" s="5" t="s">
         <v>109</v>
       </c>
@@ -2443,11 +2443,11 @@
       <c r="E63" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F63" s="37"/>
+      <c r="F63" s="26"/>
       <c r="G63" s="7"/>
     </row>
     <row r="64" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A64" s="27"/>
+      <c r="A64" s="32"/>
       <c r="B64" s="5" t="s">
         <v>61</v>
       </c>
@@ -2460,11 +2460,11 @@
       <c r="E64" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F64" s="37"/>
+      <c r="F64" s="26"/>
       <c r="G64" s="7"/>
     </row>
     <row r="65" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A65" s="27"/>
+      <c r="A65" s="32"/>
       <c r="B65" s="5" t="s">
         <v>62</v>
       </c>
@@ -2477,11 +2477,11 @@
       <c r="E65" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F65" s="37"/>
+      <c r="F65" s="26"/>
       <c r="G65" s="7"/>
     </row>
     <row r="66" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A66" s="27"/>
+      <c r="A66" s="32"/>
       <c r="B66" s="5" t="s">
         <v>63</v>
       </c>
@@ -2494,11 +2494,11 @@
       <c r="E66" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F66" s="37"/>
+      <c r="F66" s="26"/>
       <c r="G66" s="7"/>
     </row>
     <row r="67" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A67" s="27"/>
+      <c r="A67" s="32"/>
       <c r="B67" s="5" t="s">
         <v>64</v>
       </c>
@@ -2511,11 +2511,11 @@
       <c r="E67" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F67" s="37"/>
+      <c r="F67" s="26"/>
       <c r="G67" s="7"/>
     </row>
     <row r="68" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A68" s="27"/>
+      <c r="A68" s="32"/>
       <c r="B68" s="5" t="s">
         <v>65</v>
       </c>
@@ -2528,11 +2528,11 @@
       <c r="E68" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F68" s="37"/>
+      <c r="F68" s="26"/>
       <c r="G68" s="7"/>
     </row>
     <row r="69" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A69" s="27"/>
+      <c r="A69" s="32"/>
       <c r="B69" s="5" t="s">
         <v>66</v>
       </c>
@@ -2545,11 +2545,11 @@
       <c r="E69" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F69" s="37"/>
+      <c r="F69" s="26"/>
       <c r="G69" s="7"/>
     </row>
     <row r="70" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="28"/>
+      <c r="A70" s="33"/>
       <c r="B70" s="5" t="s">
         <v>67</v>
       </c>
@@ -2562,11 +2562,11 @@
       <c r="E70" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F70" s="38"/>
+      <c r="F70" s="27"/>
       <c r="G70" s="7"/>
     </row>
     <row r="71" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A71" s="30" t="s">
+      <c r="A71" s="34" t="s">
         <v>54</v>
       </c>
       <c r="B71" s="11" t="s">
@@ -2581,13 +2581,13 @@
       <c r="E71" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F71" s="36" t="s">
+      <c r="F71" s="25" t="s">
         <v>230</v>
       </c>
       <c r="G71" s="2"/>
     </row>
     <row r="72" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A72" s="31"/>
+      <c r="A72" s="35"/>
       <c r="B72" s="5" t="s">
         <v>47</v>
       </c>
@@ -2600,11 +2600,11 @@
       <c r="E72" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F72" s="37"/>
+      <c r="F72" s="26"/>
       <c r="G72" s="2"/>
     </row>
     <row r="73" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A73" s="31"/>
+      <c r="A73" s="35"/>
       <c r="B73" s="5" t="s">
         <v>6</v>
       </c>
@@ -2617,11 +2617,11 @@
       <c r="E73" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F73" s="37"/>
+      <c r="F73" s="26"/>
       <c r="G73" s="2"/>
     </row>
     <row r="74" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A74" s="31"/>
+      <c r="A74" s="35"/>
       <c r="B74" s="5" t="s">
         <v>8</v>
       </c>
@@ -2634,11 +2634,11 @@
       <c r="E74" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F74" s="37"/>
+      <c r="F74" s="26"/>
       <c r="G74" s="2"/>
     </row>
     <row r="75" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A75" s="31"/>
+      <c r="A75" s="35"/>
       <c r="B75" s="5" t="s">
         <v>48</v>
       </c>
@@ -2651,11 +2651,11 @@
       <c r="E75" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F75" s="37"/>
+      <c r="F75" s="26"/>
       <c r="G75" s="2"/>
     </row>
     <row r="76" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A76" s="31"/>
+      <c r="A76" s="35"/>
       <c r="B76" s="5" t="s">
         <v>7</v>
       </c>
@@ -2668,11 +2668,11 @@
       <c r="E76" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F76" s="37"/>
+      <c r="F76" s="26"/>
       <c r="G76" s="2"/>
     </row>
     <row r="77" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A77" s="31"/>
+      <c r="A77" s="35"/>
       <c r="B77" s="5" t="s">
         <v>16</v>
       </c>
@@ -2685,11 +2685,11 @@
       <c r="E77" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F77" s="37"/>
+      <c r="F77" s="26"/>
       <c r="G77" s="2"/>
     </row>
     <row r="78" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A78" s="31"/>
+      <c r="A78" s="35"/>
       <c r="B78" s="5" t="s">
         <v>17</v>
       </c>
@@ -2702,11 +2702,11 @@
       <c r="E78" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F78" s="37"/>
+      <c r="F78" s="26"/>
       <c r="G78" s="2"/>
     </row>
     <row r="79" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A79" s="31"/>
+      <c r="A79" s="35"/>
       <c r="B79" s="5" t="s">
         <v>49</v>
       </c>
@@ -2719,11 +2719,11 @@
       <c r="E79" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F79" s="37"/>
+      <c r="F79" s="26"/>
       <c r="G79" s="2"/>
     </row>
     <row r="80" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A80" s="31"/>
+      <c r="A80" s="35"/>
       <c r="B80" s="5" t="s">
         <v>50</v>
       </c>
@@ -2736,11 +2736,11 @@
       <c r="E80" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F80" s="37"/>
+      <c r="F80" s="26"/>
       <c r="G80" s="2"/>
     </row>
     <row r="81" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A81" s="31"/>
+      <c r="A81" s="35"/>
       <c r="B81" s="5" t="s">
         <v>51</v>
       </c>
@@ -2753,11 +2753,11 @@
       <c r="E81" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F81" s="37"/>
+      <c r="F81" s="26"/>
       <c r="G81" s="2"/>
     </row>
     <row r="82" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A82" s="31"/>
+      <c r="A82" s="35"/>
       <c r="B82" s="5" t="s">
         <v>52</v>
       </c>
@@ -2770,11 +2770,11 @@
       <c r="E82" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F82" s="37"/>
+      <c r="F82" s="26"/>
       <c r="G82" s="2"/>
     </row>
     <row r="83" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A83" s="31"/>
+      <c r="A83" s="35"/>
       <c r="B83" s="5" t="s">
         <v>53</v>
       </c>
@@ -2787,11 +2787,11 @@
       <c r="E83" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F83" s="37"/>
+      <c r="F83" s="26"/>
       <c r="G83" s="2"/>
     </row>
     <row r="84" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="32"/>
+      <c r="A84" s="36"/>
       <c r="B84" s="9" t="s">
         <v>32</v>
       </c>
@@ -2804,11 +2804,11 @@
       <c r="E84" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F84" s="38"/>
+      <c r="F84" s="27"/>
       <c r="G84" s="2"/>
     </row>
     <row r="85" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A85" s="30" t="s">
+      <c r="A85" s="34" t="s">
         <v>70</v>
       </c>
       <c r="B85" s="11" t="s">
@@ -2823,13 +2823,13 @@
       <c r="E85" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F85" s="36" t="s">
-        <v>236</v>
+      <c r="F85" s="25" t="s">
+        <v>235</v>
       </c>
       <c r="G85" s="2"/>
     </row>
     <row r="86" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A86" s="31"/>
+      <c r="A86" s="35"/>
       <c r="B86" s="5" t="s">
         <v>57</v>
       </c>
@@ -2842,11 +2842,11 @@
       <c r="E86" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F86" s="37"/>
+      <c r="F86" s="26"/>
       <c r="G86" s="2"/>
     </row>
     <row r="87" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A87" s="31"/>
+      <c r="A87" s="35"/>
       <c r="B87" s="5" t="s">
         <v>48</v>
       </c>
@@ -2859,11 +2859,11 @@
       <c r="E87" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F87" s="37"/>
+      <c r="F87" s="26"/>
       <c r="G87" s="2"/>
     </row>
     <row r="88" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A88" s="31"/>
+      <c r="A88" s="35"/>
       <c r="B88" s="5" t="s">
         <v>7</v>
       </c>
@@ -2876,11 +2876,11 @@
       <c r="E88" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F88" s="37"/>
+      <c r="F88" s="26"/>
       <c r="G88" s="2"/>
     </row>
     <row r="89" spans="1:7" ht="33" x14ac:dyDescent="0.3">
-      <c r="A89" s="31"/>
+      <c r="A89" s="35"/>
       <c r="B89" s="5" t="s">
         <v>58</v>
       </c>
@@ -2893,11 +2893,11 @@
       <c r="E89" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F89" s="37"/>
+      <c r="F89" s="26"/>
       <c r="G89" s="2"/>
     </row>
     <row r="90" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A90" s="31"/>
+      <c r="A90" s="35"/>
       <c r="B90" s="5" t="s">
         <v>59</v>
       </c>
@@ -2910,11 +2910,11 @@
       <c r="E90" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F90" s="37"/>
+      <c r="F90" s="26"/>
       <c r="G90" s="2"/>
     </row>
     <row r="91" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A91" s="31"/>
+      <c r="A91" s="35"/>
       <c r="B91" s="5" t="s">
         <v>60</v>
       </c>
@@ -2927,11 +2927,11 @@
       <c r="E91" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F91" s="37"/>
+      <c r="F91" s="26"/>
       <c r="G91" s="2"/>
     </row>
     <row r="92" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A92" s="31"/>
+      <c r="A92" s="35"/>
       <c r="B92" s="5" t="s">
         <v>61</v>
       </c>
@@ -2944,11 +2944,11 @@
       <c r="E92" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F92" s="37"/>
+      <c r="F92" s="26"/>
       <c r="G92" s="2"/>
     </row>
     <row r="93" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A93" s="31"/>
+      <c r="A93" s="35"/>
       <c r="B93" s="5" t="s">
         <v>62</v>
       </c>
@@ -2961,11 +2961,11 @@
       <c r="E93" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F93" s="37"/>
+      <c r="F93" s="26"/>
       <c r="G93" s="2"/>
     </row>
     <row r="94" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A94" s="31"/>
+      <c r="A94" s="35"/>
       <c r="B94" s="5" t="s">
         <v>63</v>
       </c>
@@ -2978,11 +2978,11 @@
       <c r="E94" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F94" s="37"/>
+      <c r="F94" s="26"/>
       <c r="G94" s="2"/>
     </row>
     <row r="95" spans="1:7" ht="33" x14ac:dyDescent="0.3">
-      <c r="A95" s="31"/>
+      <c r="A95" s="35"/>
       <c r="B95" s="5" t="s">
         <v>64</v>
       </c>
@@ -2995,11 +2995,11 @@
       <c r="E95" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F95" s="37"/>
+      <c r="F95" s="26"/>
       <c r="G95" s="2"/>
     </row>
     <row r="96" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A96" s="31"/>
+      <c r="A96" s="35"/>
       <c r="B96" s="5" t="s">
         <v>65</v>
       </c>
@@ -3012,11 +3012,11 @@
       <c r="E96" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F96" s="37"/>
+      <c r="F96" s="26"/>
       <c r="G96" s="2"/>
     </row>
     <row r="97" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A97" s="31"/>
+      <c r="A97" s="35"/>
       <c r="B97" s="5" t="s">
         <v>66</v>
       </c>
@@ -3029,11 +3029,11 @@
       <c r="E97" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F97" s="37"/>
+      <c r="F97" s="26"/>
       <c r="G97" s="2"/>
     </row>
     <row r="98" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="32"/>
+      <c r="A98" s="36"/>
       <c r="B98" s="9" t="s">
         <v>67</v>
       </c>
@@ -3046,11 +3046,11 @@
       <c r="E98" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F98" s="38"/>
+      <c r="F98" s="27"/>
       <c r="G98" s="2"/>
     </row>
     <row r="99" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A99" s="39" t="s">
+      <c r="A99" s="28" t="s">
         <v>80</v>
       </c>
       <c r="B99" s="11" t="s">
@@ -3065,13 +3065,13 @@
       <c r="E99" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F99" s="36" t="s">
+      <c r="F99" s="25" t="s">
         <v>139</v>
       </c>
       <c r="G99" s="2"/>
     </row>
     <row r="100" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A100" s="40"/>
+      <c r="A100" s="29"/>
       <c r="B100" s="5" t="s">
         <v>48</v>
       </c>
@@ -3084,11 +3084,11 @@
       <c r="E100" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F100" s="37"/>
+      <c r="F100" s="26"/>
       <c r="G100" s="2"/>
     </row>
     <row r="101" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A101" s="40"/>
+      <c r="A101" s="29"/>
       <c r="B101" s="5" t="s">
         <v>7</v>
       </c>
@@ -3101,11 +3101,11 @@
       <c r="E101" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F101" s="37"/>
+      <c r="F101" s="26"/>
       <c r="G101" s="2"/>
     </row>
     <row r="102" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A102" s="40"/>
+      <c r="A102" s="29"/>
       <c r="B102" s="5" t="s">
         <v>5</v>
       </c>
@@ -3118,11 +3118,11 @@
       <c r="E102" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F102" s="37"/>
+      <c r="F102" s="26"/>
       <c r="G102" s="2"/>
     </row>
     <row r="103" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A103" s="40"/>
+      <c r="A103" s="29"/>
       <c r="B103" s="5" t="s">
         <v>72</v>
       </c>
@@ -3135,11 +3135,11 @@
       <c r="E103" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F103" s="37"/>
+      <c r="F103" s="26"/>
       <c r="G103" s="2"/>
     </row>
     <row r="104" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A104" s="40"/>
+      <c r="A104" s="29"/>
       <c r="B104" s="5" t="s">
         <v>73</v>
       </c>
@@ -3152,11 +3152,11 @@
       <c r="E104" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F104" s="37"/>
+      <c r="F104" s="26"/>
       <c r="G104" s="2"/>
     </row>
     <row r="105" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A105" s="40"/>
+      <c r="A105" s="29"/>
       <c r="B105" s="5" t="s">
         <v>14</v>
       </c>
@@ -3169,11 +3169,11 @@
       <c r="E105" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F105" s="37"/>
+      <c r="F105" s="26"/>
       <c r="G105" s="2"/>
     </row>
     <row r="106" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A106" s="40"/>
+      <c r="A106" s="29"/>
       <c r="B106" s="5" t="s">
         <v>15</v>
       </c>
@@ -3186,11 +3186,11 @@
       <c r="E106" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F106" s="37"/>
+      <c r="F106" s="26"/>
       <c r="G106" s="2"/>
     </row>
     <row r="107" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A107" s="40"/>
+      <c r="A107" s="29"/>
       <c r="B107" s="5" t="s">
         <v>16</v>
       </c>
@@ -3203,11 +3203,11 @@
       <c r="E107" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F107" s="37"/>
+      <c r="F107" s="26"/>
       <c r="G107" s="2"/>
     </row>
     <row r="108" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A108" s="40"/>
+      <c r="A108" s="29"/>
       <c r="B108" s="5" t="s">
         <v>17</v>
       </c>
@@ -3220,11 +3220,11 @@
       <c r="E108" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F108" s="37"/>
+      <c r="F108" s="26"/>
       <c r="G108" s="2"/>
     </row>
     <row r="109" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A109" s="40"/>
+      <c r="A109" s="29"/>
       <c r="B109" s="5" t="s">
         <v>46</v>
       </c>
@@ -3237,11 +3237,11 @@
       <c r="E109" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F109" s="37"/>
+      <c r="F109" s="26"/>
       <c r="G109" s="2"/>
     </row>
     <row r="110" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A110" s="40"/>
+      <c r="A110" s="29"/>
       <c r="B110" s="5" t="s">
         <v>32</v>
       </c>
@@ -3254,11 +3254,11 @@
       <c r="E110" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F110" s="37"/>
+      <c r="F110" s="26"/>
       <c r="G110" s="2"/>
     </row>
     <row r="111" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A111" s="40"/>
+      <c r="A111" s="29"/>
       <c r="B111" s="5" t="s">
         <v>74</v>
       </c>
@@ -3271,11 +3271,11 @@
       <c r="E111" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F111" s="37"/>
+      <c r="F111" s="26"/>
       <c r="G111" s="2"/>
     </row>
     <row r="112" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A112" s="40"/>
+      <c r="A112" s="29"/>
       <c r="B112" s="5" t="s">
         <v>75</v>
       </c>
@@ -3288,11 +3288,11 @@
       <c r="E112" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F112" s="37"/>
+      <c r="F112" s="26"/>
       <c r="G112" s="2"/>
     </row>
     <row r="113" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A113" s="40"/>
+      <c r="A113" s="29"/>
       <c r="B113" s="5" t="s">
         <v>76</v>
       </c>
@@ -3305,11 +3305,11 @@
       <c r="E113" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F113" s="37"/>
+      <c r="F113" s="26"/>
       <c r="G113" s="2"/>
     </row>
     <row r="114" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A114" s="40"/>
+      <c r="A114" s="29"/>
       <c r="B114" s="5" t="s">
         <v>77</v>
       </c>
@@ -3322,11 +3322,11 @@
       <c r="E114" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F114" s="37"/>
+      <c r="F114" s="26"/>
       <c r="G114" s="2"/>
     </row>
     <row r="115" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A115" s="40"/>
+      <c r="A115" s="29"/>
       <c r="B115" s="5" t="s">
         <v>78</v>
       </c>
@@ -3339,11 +3339,11 @@
       <c r="E115" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F115" s="37"/>
+      <c r="F115" s="26"/>
       <c r="G115" s="2"/>
     </row>
     <row r="116" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="41"/>
+      <c r="A116" s="30"/>
       <c r="B116" s="9" t="s">
         <v>79</v>
       </c>
@@ -3356,11 +3356,11 @@
       <c r="E116" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F116" s="38"/>
+      <c r="F116" s="27"/>
       <c r="G116" s="2"/>
     </row>
     <row r="117" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A117" s="39" t="s">
+      <c r="A117" s="28" t="s">
         <v>85</v>
       </c>
       <c r="B117" s="11" t="s">
@@ -3375,13 +3375,13 @@
       <c r="E117" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F117" s="36" t="s">
+      <c r="F117" s="25" t="s">
         <v>131</v>
       </c>
       <c r="G117" s="2"/>
     </row>
     <row r="118" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A118" s="40"/>
+      <c r="A118" s="29"/>
       <c r="B118" s="5" t="s">
         <v>57</v>
       </c>
@@ -3394,11 +3394,11 @@
       <c r="E118" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F118" s="37"/>
+      <c r="F118" s="26"/>
       <c r="G118" s="2"/>
     </row>
     <row r="119" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A119" s="40"/>
+      <c r="A119" s="29"/>
       <c r="B119" s="5" t="s">
         <v>48</v>
       </c>
@@ -3411,11 +3411,11 @@
       <c r="E119" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F119" s="37"/>
+      <c r="F119" s="26"/>
       <c r="G119" s="2"/>
     </row>
     <row r="120" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A120" s="40"/>
+      <c r="A120" s="29"/>
       <c r="B120" s="5" t="s">
         <v>7</v>
       </c>
@@ -3428,11 +3428,11 @@
       <c r="E120" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F120" s="37"/>
+      <c r="F120" s="26"/>
       <c r="G120" s="2"/>
     </row>
     <row r="121" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A121" s="40"/>
+      <c r="A121" s="29"/>
       <c r="B121" s="5" t="s">
         <v>46</v>
       </c>
@@ -3445,11 +3445,11 @@
       <c r="E121" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F121" s="37"/>
+      <c r="F121" s="26"/>
       <c r="G121" s="2"/>
     </row>
     <row r="122" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A122" s="40"/>
+      <c r="A122" s="29"/>
       <c r="B122" s="5" t="s">
         <v>5</v>
       </c>
@@ -3462,11 +3462,11 @@
       <c r="E122" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F122" s="37"/>
+      <c r="F122" s="26"/>
       <c r="G122" s="2"/>
     </row>
     <row r="123" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A123" s="40"/>
+      <c r="A123" s="29"/>
       <c r="B123" s="5" t="s">
         <v>25</v>
       </c>
@@ -3479,11 +3479,11 @@
       <c r="E123" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F123" s="37"/>
+      <c r="F123" s="26"/>
       <c r="G123" s="2"/>
     </row>
     <row r="124" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A124" s="40"/>
+      <c r="A124" s="29"/>
       <c r="B124" s="5" t="s">
         <v>81</v>
       </c>
@@ -3496,11 +3496,11 @@
       <c r="E124" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F124" s="37"/>
+      <c r="F124" s="26"/>
       <c r="G124" s="2"/>
     </row>
     <row r="125" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A125" s="40"/>
+      <c r="A125" s="29"/>
       <c r="B125" s="5" t="s">
         <v>72</v>
       </c>
@@ -3513,11 +3513,11 @@
       <c r="E125" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F125" s="37"/>
+      <c r="F125" s="26"/>
       <c r="G125" s="2"/>
     </row>
     <row r="126" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A126" s="40"/>
+      <c r="A126" s="29"/>
       <c r="B126" s="5" t="s">
         <v>73</v>
       </c>
@@ -3530,11 +3530,11 @@
       <c r="E126" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F126" s="37"/>
+      <c r="F126" s="26"/>
       <c r="G126" s="2"/>
     </row>
     <row r="127" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A127" s="40"/>
+      <c r="A127" s="29"/>
       <c r="B127" s="5" t="s">
         <v>13</v>
       </c>
@@ -3547,11 +3547,11 @@
       <c r="E127" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F127" s="37"/>
+      <c r="F127" s="26"/>
       <c r="G127" s="2"/>
     </row>
     <row r="128" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A128" s="40"/>
+      <c r="A128" s="29"/>
       <c r="B128" s="5" t="s">
         <v>14</v>
       </c>
@@ -3564,11 +3564,11 @@
       <c r="E128" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F128" s="37"/>
+      <c r="F128" s="26"/>
       <c r="G128" s="2"/>
     </row>
     <row r="129" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A129" s="40"/>
+      <c r="A129" s="29"/>
       <c r="B129" s="5" t="s">
         <v>15</v>
       </c>
@@ -3581,11 +3581,11 @@
       <c r="E129" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F129" s="37"/>
+      <c r="F129" s="26"/>
       <c r="G129" s="2"/>
     </row>
     <row r="130" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A130" s="40"/>
+      <c r="A130" s="29"/>
       <c r="B130" s="5" t="s">
         <v>16</v>
       </c>
@@ -3598,11 +3598,11 @@
       <c r="E130" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F130" s="37"/>
+      <c r="F130" s="26"/>
       <c r="G130" s="2"/>
     </row>
     <row r="131" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A131" s="40"/>
+      <c r="A131" s="29"/>
       <c r="B131" s="5" t="s">
         <v>17</v>
       </c>
@@ -3615,11 +3615,11 @@
       <c r="E131" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F131" s="37"/>
+      <c r="F131" s="26"/>
       <c r="G131" s="2"/>
     </row>
     <row r="132" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A132" s="40"/>
+      <c r="A132" s="29"/>
       <c r="B132" s="5" t="s">
         <v>8</v>
       </c>
@@ -3632,11 +3632,11 @@
       <c r="E132" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F132" s="37"/>
+      <c r="F132" s="26"/>
       <c r="G132" s="2"/>
     </row>
     <row r="133" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A133" s="40"/>
+      <c r="A133" s="29"/>
       <c r="B133" s="5" t="s">
         <v>82</v>
       </c>
@@ -3649,11 +3649,11 @@
       <c r="E133" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F133" s="37"/>
+      <c r="F133" s="26"/>
       <c r="G133" s="2"/>
     </row>
     <row r="134" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A134" s="40"/>
+      <c r="A134" s="29"/>
       <c r="B134" s="5" t="s">
         <v>35</v>
       </c>
@@ -3666,11 +3666,11 @@
       <c r="E134" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F134" s="37"/>
+      <c r="F134" s="26"/>
       <c r="G134" s="2"/>
     </row>
     <row r="135" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A135" s="40"/>
+      <c r="A135" s="29"/>
       <c r="B135" s="5" t="s">
         <v>83</v>
       </c>
@@ -3683,11 +3683,11 @@
       <c r="E135" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F135" s="37"/>
+      <c r="F135" s="26"/>
       <c r="G135" s="2"/>
     </row>
     <row r="136" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A136" s="40"/>
+      <c r="A136" s="29"/>
       <c r="B136" s="5" t="s">
         <v>84</v>
       </c>
@@ -3700,11 +3700,11 @@
       <c r="E136" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F136" s="37"/>
+      <c r="F136" s="26"/>
       <c r="G136" s="2"/>
     </row>
     <row r="137" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="41"/>
+      <c r="A137" s="30"/>
       <c r="B137" s="9" t="s">
         <v>32</v>
       </c>
@@ -3717,11 +3717,17 @@
       <c r="E137" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F137" s="38"/>
+      <c r="F137" s="27"/>
       <c r="G137" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="A17:A34"/>
+    <mergeCell ref="A35:A47"/>
+    <mergeCell ref="A71:A84"/>
+    <mergeCell ref="F3:F16"/>
     <mergeCell ref="F117:F137"/>
     <mergeCell ref="F99:F116"/>
     <mergeCell ref="A99:A116"/>
@@ -3735,12 +3741,6 @@
     <mergeCell ref="F85:F98"/>
     <mergeCell ref="F71:F84"/>
     <mergeCell ref="A85:A98"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:A16"/>
-    <mergeCell ref="A17:A34"/>
-    <mergeCell ref="A35:A47"/>
-    <mergeCell ref="A71:A84"/>
-    <mergeCell ref="F3:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3751,8 +3751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3766,14 +3766,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3796,7 +3796,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="38" t="s">
         <v>233</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -3811,12 +3811,12 @@
       <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="33" t="s">
-        <v>235</v>
+      <c r="F3" s="39" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="27"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
@@ -3829,10 +3829,10 @@
       <c r="E4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="34"/>
+      <c r="F4" s="40"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
@@ -3845,10 +3845,10 @@
       <c r="E5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="34"/>
+      <c r="F5" s="40"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="27"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="5" t="s">
         <v>142</v>
       </c>
@@ -3861,10 +3861,10 @@
       <c r="E6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="40"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="5" t="s">
         <v>143</v>
       </c>
@@ -3877,10 +3877,10 @@
       <c r="E7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="28"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="9" t="s">
         <v>144</v>
       </c>
@@ -3893,10 +3893,10 @@
       <c r="E8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="35"/>
+      <c r="F8" s="41"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="42" t="s">
         <v>150</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -3911,12 +3911,12 @@
       <c r="E9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="25" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="5" t="s">
         <v>147</v>
       </c>
@@ -3929,10 +3929,10 @@
       <c r="E10" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F10" s="37"/>
+      <c r="F10" s="26"/>
     </row>
     <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="46"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="5" t="s">
         <v>148</v>
       </c>
@@ -3945,10 +3945,10 @@
       <c r="E11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="37"/>
+      <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
@@ -3961,10 +3961,10 @@
       <c r="E12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="37"/>
+      <c r="F12" s="26"/>
     </row>
     <row r="13" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A13" s="46"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -3977,10 +3977,10 @@
       <c r="E13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="37"/>
+      <c r="F13" s="26"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="46"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
@@ -3993,10 +3993,10 @@
       <c r="E14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="37"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="47"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="9" t="s">
         <v>149</v>
       </c>
@@ -4009,10 +4009,10 @@
       <c r="E15" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="F15" s="38"/>
+      <c r="F15" s="27"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="31" t="s">
         <v>234</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -4025,12 +4025,12 @@
       <c r="E16" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="45" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="5" t="s">
         <v>6</v>
       </c>
@@ -4043,10 +4043,10 @@
       <c r="E17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="34"/>
+      <c r="F17" s="40"/>
     </row>
     <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="5" t="s">
         <v>158</v>
       </c>
@@ -4059,10 +4059,10 @@
       <c r="E18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="34"/>
+      <c r="F18" s="40"/>
     </row>
     <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="27"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="5" t="s">
         <v>159</v>
       </c>
@@ -4075,10 +4075,10 @@
       <c r="E19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="34"/>
+      <c r="F19" s="40"/>
     </row>
     <row r="20" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="28"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="9" t="s">
         <v>144</v>
       </c>
@@ -4091,10 +4091,10 @@
       <c r="E20" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="35"/>
+      <c r="F20" s="41"/>
     </row>
     <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="45" t="s">
         <v>202</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -4109,12 +4109,12 @@
       <c r="E21" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="F21" s="36" t="s">
+      <c r="F21" s="25" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="34"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="5" t="s">
         <v>167</v>
       </c>
@@ -4127,10 +4127,10 @@
       <c r="E22" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="26"/>
     </row>
     <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="34"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="5" t="s">
         <v>172</v>
       </c>
@@ -4143,10 +4143,10 @@
       <c r="E23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="37"/>
+      <c r="F23" s="26"/>
     </row>
     <row r="24" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="34"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="5" t="s">
         <v>190</v>
       </c>
@@ -4159,10 +4159,10 @@
       <c r="E24" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="37"/>
+      <c r="F24" s="26"/>
     </row>
     <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="34"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="5" t="s">
         <v>191</v>
       </c>
@@ -4175,10 +4175,10 @@
       <c r="E25" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="F25" s="37"/>
+      <c r="F25" s="26"/>
     </row>
     <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="34"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="5" t="s">
         <v>192</v>
       </c>
@@ -4191,10 +4191,10 @@
       <c r="E26" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="F26" s="37"/>
+      <c r="F26" s="26"/>
     </row>
     <row r="27" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="34"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="5" t="s">
         <v>193</v>
       </c>
@@ -4207,10 +4207,10 @@
       <c r="E27" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="F27" s="37"/>
+      <c r="F27" s="26"/>
     </row>
     <row r="28" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="34"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="5" t="s">
         <v>194</v>
       </c>
@@ -4223,10 +4223,10 @@
       <c r="E28" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F28" s="37"/>
+      <c r="F28" s="26"/>
     </row>
     <row r="29" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="34"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="5" t="s">
         <v>195</v>
       </c>
@@ -4239,10 +4239,10 @@
       <c r="E29" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="37"/>
+      <c r="F29" s="26"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="34"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="5" t="s">
         <v>169</v>
       </c>
@@ -4255,10 +4255,10 @@
       <c r="E30" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="37"/>
+      <c r="F30" s="26"/>
     </row>
     <row r="31" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="34"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="5" t="s">
         <v>170</v>
       </c>
@@ -4271,10 +4271,10 @@
       <c r="E31" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="37"/>
+      <c r="F31" s="26"/>
     </row>
     <row r="32" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="34"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="5" t="s">
         <v>196</v>
       </c>
@@ -4287,10 +4287,10 @@
       <c r="E32" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F32" s="37"/>
+      <c r="F32" s="26"/>
     </row>
     <row r="33" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="34"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="5" t="s">
         <v>197</v>
       </c>
@@ -4303,10 +4303,10 @@
       <c r="E33" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F33" s="37"/>
+      <c r="F33" s="26"/>
     </row>
     <row r="34" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="34"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="5" t="s">
         <v>198</v>
       </c>
@@ -4319,10 +4319,10 @@
       <c r="E34" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F34" s="37"/>
+      <c r="F34" s="26"/>
     </row>
     <row r="35" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="35"/>
+      <c r="A35" s="41"/>
       <c r="B35" s="9" t="s">
         <v>199</v>
       </c>
@@ -4335,10 +4335,10 @@
       <c r="E35" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="F35" s="38"/>
+      <c r="F35" s="27"/>
     </row>
     <row r="36" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="45" t="s">
         <v>166</v>
       </c>
       <c r="B36" s="11" t="s">
@@ -4347,88 +4347,88 @@
       <c r="C36" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D36" s="43" t="s">
+      <c r="D36" s="46" t="s">
         <v>222</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="F36" s="36" t="s">
+      <c r="F36" s="25" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="34"/>
+      <c r="A37" s="40"/>
       <c r="B37" s="5" t="s">
         <v>168</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D37" s="44"/>
+      <c r="D37" s="47"/>
       <c r="E37" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F37" s="37"/>
+      <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="34"/>
+      <c r="A38" s="40"/>
       <c r="B38" s="5" t="s">
         <v>169</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="44"/>
+      <c r="D38" s="47"/>
       <c r="E38" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="37"/>
+      <c r="F38" s="26"/>
     </row>
     <row r="39" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="34"/>
+      <c r="A39" s="40"/>
       <c r="B39" s="5" t="s">
         <v>170</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="44"/>
+      <c r="D39" s="47"/>
       <c r="E39" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="37"/>
+      <c r="F39" s="26"/>
     </row>
     <row r="40" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="34"/>
+      <c r="A40" s="40"/>
       <c r="B40" s="5" t="s">
         <v>171</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="44"/>
+      <c r="D40" s="47"/>
       <c r="E40" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F40" s="37"/>
+      <c r="F40" s="26"/>
     </row>
     <row r="41" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="34"/>
+      <c r="A41" s="40"/>
       <c r="B41" s="5" t="s">
         <v>172</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D41" s="44"/>
+      <c r="D41" s="47"/>
       <c r="E41" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F41" s="37"/>
+      <c r="F41" s="26"/>
     </row>
     <row r="42" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="34"/>
+      <c r="A42" s="40"/>
       <c r="B42" s="5" t="s">
         <v>173</v>
       </c>
@@ -4439,10 +4439,10 @@
       <c r="E42" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F42" s="37"/>
+      <c r="F42" s="26"/>
     </row>
     <row r="43" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="34"/>
+      <c r="A43" s="40"/>
       <c r="B43" s="5" t="s">
         <v>174</v>
       </c>
@@ -4453,10 +4453,10 @@
       <c r="E43" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F43" s="37"/>
+      <c r="F43" s="26"/>
     </row>
     <row r="44" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A44" s="34"/>
+      <c r="A44" s="40"/>
       <c r="B44" s="5" t="s">
         <v>175</v>
       </c>
@@ -4469,10 +4469,10 @@
       <c r="E44" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F44" s="37"/>
+      <c r="F44" s="26"/>
     </row>
     <row r="45" spans="1:6" ht="66" x14ac:dyDescent="0.3">
-      <c r="A45" s="34"/>
+      <c r="A45" s="40"/>
       <c r="B45" s="5" t="s">
         <v>176</v>
       </c>
@@ -4485,10 +4485,10 @@
       <c r="E45" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F45" s="37"/>
+      <c r="F45" s="26"/>
     </row>
     <row r="46" spans="1:6" ht="66" x14ac:dyDescent="0.3">
-      <c r="A46" s="34"/>
+      <c r="A46" s="40"/>
       <c r="B46" s="5" t="s">
         <v>177</v>
       </c>
@@ -4501,10 +4501,10 @@
       <c r="E46" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F46" s="37"/>
+      <c r="F46" s="26"/>
     </row>
     <row r="47" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A47" s="34"/>
+      <c r="A47" s="40"/>
       <c r="B47" s="5" t="s">
         <v>161</v>
       </c>
@@ -4517,10 +4517,10 @@
       <c r="E47" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F47" s="37"/>
+      <c r="F47" s="26"/>
     </row>
     <row r="48" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A48" s="34"/>
+      <c r="A48" s="40"/>
       <c r="B48" s="5" t="s">
         <v>178</v>
       </c>
@@ -4533,10 +4533,10 @@
       <c r="E48" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F48" s="37"/>
+      <c r="F48" s="26"/>
     </row>
     <row r="49" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A49" s="34"/>
+      <c r="A49" s="40"/>
       <c r="B49" s="5" t="s">
         <v>179</v>
       </c>
@@ -4549,10 +4549,10 @@
       <c r="E49" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F49" s="37"/>
+      <c r="F49" s="26"/>
     </row>
     <row r="50" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A50" s="34"/>
+      <c r="A50" s="40"/>
       <c r="B50" s="5" t="s">
         <v>180</v>
       </c>
@@ -4565,10 +4565,10 @@
       <c r="E50" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F50" s="37"/>
+      <c r="F50" s="26"/>
     </row>
     <row r="51" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A51" s="34"/>
+      <c r="A51" s="40"/>
       <c r="B51" s="5" t="s">
         <v>181</v>
       </c>
@@ -4581,10 +4581,10 @@
       <c r="E51" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F51" s="37"/>
+      <c r="F51" s="26"/>
     </row>
     <row r="52" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A52" s="34"/>
+      <c r="A52" s="40"/>
       <c r="B52" s="5" t="s">
         <v>182</v>
       </c>
@@ -4597,10 +4597,10 @@
       <c r="E52" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F52" s="37"/>
+      <c r="F52" s="26"/>
     </row>
     <row r="53" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A53" s="34"/>
+      <c r="A53" s="40"/>
       <c r="B53" s="5" t="s">
         <v>183</v>
       </c>
@@ -4611,10 +4611,10 @@
       <c r="E53" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F53" s="37"/>
+      <c r="F53" s="26"/>
     </row>
     <row r="54" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="34"/>
+      <c r="A54" s="40"/>
       <c r="B54" s="5" t="s">
         <v>184</v>
       </c>
@@ -4627,10 +4627,10 @@
       <c r="E54" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F54" s="37"/>
+      <c r="F54" s="26"/>
     </row>
     <row r="55" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A55" s="34"/>
+      <c r="A55" s="40"/>
       <c r="B55" s="5" t="s">
         <v>185</v>
       </c>
@@ -4643,10 +4643,10 @@
       <c r="E55" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F55" s="37"/>
+      <c r="F55" s="26"/>
     </row>
     <row r="56" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="34"/>
+      <c r="A56" s="40"/>
       <c r="B56" s="5" t="s">
         <v>186</v>
       </c>
@@ -4659,10 +4659,10 @@
       <c r="E56" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F56" s="37"/>
+      <c r="F56" s="26"/>
     </row>
     <row r="57" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A57" s="34"/>
+      <c r="A57" s="40"/>
       <c r="B57" s="5" t="s">
         <v>187</v>
       </c>
@@ -4675,10 +4675,10 @@
       <c r="E57" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F57" s="37"/>
+      <c r="F57" s="26"/>
     </row>
     <row r="58" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A58" s="34"/>
+      <c r="A58" s="40"/>
       <c r="B58" s="5" t="s">
         <v>188</v>
       </c>
@@ -4689,10 +4689,10 @@
       <c r="E58" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F58" s="37"/>
+      <c r="F58" s="26"/>
     </row>
     <row r="59" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="35"/>
+      <c r="A59" s="41"/>
       <c r="B59" s="9" t="s">
         <v>189</v>
       </c>
@@ -4705,10 +4705,15 @@
       <c r="E59" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F59" s="38"/>
+      <c r="F59" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A21:A35"/>
+    <mergeCell ref="F21:F35"/>
+    <mergeCell ref="A36:A59"/>
+    <mergeCell ref="D36:D41"/>
+    <mergeCell ref="F36:F59"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A9:A15"/>
@@ -4716,11 +4721,6 @@
     <mergeCell ref="F16:F20"/>
     <mergeCell ref="F3:F8"/>
     <mergeCell ref="F9:F15"/>
-    <mergeCell ref="A21:A35"/>
-    <mergeCell ref="F21:F35"/>
-    <mergeCell ref="A36:A59"/>
-    <mergeCell ref="D36:D41"/>
-    <mergeCell ref="F36:F59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>